<commit_message>
new combination in excel results for geneva
</commit_message>
<xml_diff>
--- a/Data/Simulation Results.xlsx
+++ b/Data/Simulation Results.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Total (kWh)</t>
   </si>
@@ -84,10 +84,13 @@
     <t>Madrid</t>
   </si>
   <si>
-    <t>Adaptive Solar Facade</t>
-  </si>
-  <si>
     <t>Geneva</t>
+  </si>
+  <si>
+    <t>Adaptive Solar Facade (2 Clusters, 3*6 angles)</t>
+  </si>
+  <si>
+    <t>Adaptive Solar Facade (1 Cluster, 3*12 angles)</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -641,8 +644,8 @@
     <col min="1" max="1" width="31.25" customWidth="1"/>
     <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="41.625" customWidth="1"/>
+    <col min="5" max="5" width="40.625" customWidth="1"/>
     <col min="6" max="6" width="34.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -654,9 +657,11 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,7 +793,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,8 +809,11 @@
       <c r="D16">
         <v>441.89</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>442.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -818,8 +826,11 @@
       <c r="D17">
         <v>488.33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>504.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -832,8 +843,11 @@
       <c r="D18">
         <v>432.43</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>432.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -846,11 +860,14 @@
       <c r="D19" s="1">
         <v>1362.65</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>1379.09</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>

</xml_diff>